<commit_message>
edit table proxy and add functional for parser
</commit_message>
<xml_diff>
--- a/app/upload_file/string_дляпарсинг.xlsx
+++ b/app/upload_file/string_дляпарсинг.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_.programming\emex_autosturktura\app\api_v1\parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Артикул</t>
   </si>
@@ -65,25 +65,10 @@
     <t>254.86</t>
   </si>
   <si>
-    <t>00004254A2</t>
-  </si>
-  <si>
-    <t>6100.98</t>
-  </si>
-  <si>
     <t>Peugeot---Citroen</t>
   </si>
   <si>
     <t>Mahle---Knecht</t>
-  </si>
-  <si>
-    <t>ГАЗ</t>
-  </si>
-  <si>
-    <t>00008120T7</t>
-  </si>
-  <si>
-    <t>00006426YN</t>
   </si>
   <si>
     <t>02943N0</t>
@@ -421,7 +406,7 @@
   <dimension ref="A1:K217"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:G217"/>
+      <selection activeCell="A5" sqref="A4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,10 +454,10 @@
         <v>82026</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2">
         <v>82026</v>
@@ -493,16 +478,16 @@
     </row>
     <row r="3" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -519,135 +504,65 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>362312</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2">
-        <v>362312</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>6270000290</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2">
-        <v>6270000290</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>

</xml_diff>